<commit_message>
more work on manual normalization calculation
</commit_message>
<xml_diff>
--- a/Assets/stockParts.xlsx
+++ b/Assets/stockParts.xlsx
@@ -1492,358 +1492,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="42">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2175,7 +1824,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G29" sqref="G29"/>
+      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2282,6 +1931,9 @@
       <c r="F3">
         <v>120</v>
       </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
       <c r="H3" t="b">
         <v>0</v>
       </c>
@@ -2302,6 +1954,15 @@
       <c r="D4" t="b">
         <v>1</v>
       </c>
+      <c r="E4">
+        <v>180</v>
+      </c>
+      <c r="F4">
+        <v>100</v>
+      </c>
+      <c r="G4">
+        <v>26</v>
+      </c>
       <c r="H4" t="b">
         <v>0</v>
       </c>
@@ -2525,6 +2186,15 @@
       <c r="D12" t="b">
         <v>1</v>
       </c>
+      <c r="E12">
+        <v>127</v>
+      </c>
+      <c r="F12">
+        <v>63</v>
+      </c>
+      <c r="G12">
+        <v>138</v>
+      </c>
       <c r="H12" t="b">
         <v>0</v>
       </c>
@@ -2545,6 +2215,15 @@
       <c r="D13" t="b">
         <v>1</v>
       </c>
+      <c r="E13">
+        <v>183</v>
+      </c>
+      <c r="F13">
+        <v>63</v>
+      </c>
+      <c r="G13">
+        <v>88</v>
+      </c>
       <c r="H13" t="b">
         <v>0</v>
       </c>
@@ -2565,6 +2244,15 @@
       <c r="D14" t="b">
         <v>1</v>
       </c>
+      <c r="E14">
+        <v>183</v>
+      </c>
+      <c r="F14">
+        <v>63</v>
+      </c>
+      <c r="G14">
+        <v>88</v>
+      </c>
       <c r="H14" t="b">
         <v>0</v>
       </c>
@@ -2900,6 +2588,15 @@
       </c>
       <c r="D29" t="b">
         <v>1</v>
+      </c>
+      <c r="E29">
+        <v>208</v>
+      </c>
+      <c r="F29">
+        <v>150</v>
+      </c>
+      <c r="G29">
+        <v>50</v>
       </c>
       <c r="H29" t="b">
         <v>0</v>
@@ -8631,13 +8328,13 @@
     <sortCondition ref="A2:A305"/>
   </sortState>
   <conditionalFormatting sqref="L1 B1:I1048576">
-    <cfRule type="containsBlanks" dxfId="41" priority="1">
+    <cfRule type="containsBlanks" dxfId="2" priority="1">
       <formula>LEN(TRIM(B1))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>